<commit_message>
working on Utilities page
</commit_message>
<xml_diff>
--- a/src/main/java/utilities/Storage.xlsx
+++ b/src/main/java/utilities/Storage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santosh\Downloads\SSP\src\main\java\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F950EFF-5118-43CA-B8FC-1A5188C249B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F03C4D-A445-4B7C-A8F9-03E80818DA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="6" activeTab="9" xr2:uid="{F608F328-1BE6-4027-B2BD-9857256CBA6C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="3" xr2:uid="{F608F328-1BE6-4027-B2BD-9857256CBA6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Zone" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
   <si>
     <t>Sl.no</t>
   </si>
@@ -59,9 +59,6 @@
     <t>OSType</t>
   </si>
   <si>
-    <t>Windows</t>
-  </si>
-  <si>
     <t>TypeName</t>
   </si>
   <si>
@@ -83,10 +80,19 @@
     <t>TotalSize</t>
   </si>
   <si>
-    <t>200</t>
-  </si>
-  <si>
     <t>NameToView</t>
+  </si>
+  <si>
+    <t>Storage_16_HS</t>
+  </si>
+  <si>
+    <t>Linux</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>AutomationStorage3</t>
   </si>
 </sst>
 </file>
@@ -492,6 +498,99 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F850C7-EE77-45F3-923C-7B53248121BD}">
   <dimension ref="A1:B2"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243D4A0A-292E-4CCE-88E8-EAF8D74B89D7}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{557D6A74-48FB-4E9D-8C12-8275EC42D2DC}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C562F16-8732-4203-8130-61ADC8294938}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
@@ -503,7 +602,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -511,100 +610,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243D4A0A-292E-4CCE-88E8-EAF8D74B89D7}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{557D6A74-48FB-4E9D-8C12-8275EC42D2DC}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C562F16-8732-4203-8130-61ADC8294938}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -627,7 +633,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -655,15 +661,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -686,7 +692,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -694,7 +700,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -717,7 +723,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -725,7 +731,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -749,7 +755,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -757,7 +763,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>